<commit_message>
Proyecto 1 completado documentación añadida
</commit_message>
<xml_diff>
--- a/Documentacion/Tabla Automata.xlsx
+++ b/Documentacion/Tabla Automata.xlsx
@@ -743,9 +743,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -754,6 +751,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,15 +891,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>99219</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>29766</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>701151</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>164326</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>214979</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>119696</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -916,8 +916,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9121588" y="649941"/>
-          <a:ext cx="5620534" cy="1829055"/>
+          <a:off x="9227344" y="674688"/>
+          <a:ext cx="4282948" cy="1369852"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1422,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE55" sqref="AE55"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,27 +1440,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="F1" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="F1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="6"/>
       <c r="V1" s="1"/>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="V2" s="1"/>
@@ -1501,7 +1501,7 @@
       <c r="E4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -1530,7 +1530,7 @@
       <c r="AC4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AD4" s="21" t="s">
+      <c r="AD4" s="20" t="s">
         <v>9</v>
       </c>
       <c r="AE4" s="12" t="s">
@@ -1551,7 +1551,7 @@
       <c r="AJ4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AK4" s="21" t="s">
+      <c r="AK4" s="20" t="s">
         <v>17</v>
       </c>
       <c r="AL4" s="12" t="s">
@@ -1619,7 +1619,7 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="V5" s="1" t="s">
@@ -1690,7 +1690,7 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="V6" s="1"/>
@@ -1714,7 +1714,7 @@
       <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="V7" s="1" t="s">
@@ -1767,7 +1767,7 @@
       <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="V8" s="1"/>
@@ -1788,7 +1788,7 @@
       <c r="C9" s="3">
         <v>90</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="V9" s="1"/>
@@ -1812,7 +1812,7 @@
       <c r="C10" s="3">
         <v>90</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="V10" s="1"/>
@@ -1836,7 +1836,7 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1864,7 +1864,7 @@
       <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="F12" s="20"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="V12" s="1"/>
@@ -1885,7 +1885,7 @@
       <c r="C13" s="3">
         <v>90</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="V13" s="1"/>
@@ -1906,7 +1906,7 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="F14" s="20"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="V14" s="1"/>
@@ -1930,7 +1930,7 @@
       <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>44</v>
       </c>
       <c r="G15" s="3">
@@ -1957,7 +1957,7 @@
       <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="19" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="3">
@@ -1984,7 +1984,7 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="V17" s="1"/>
@@ -2005,7 +2005,7 @@
       <c r="C18" s="3">
         <v>90</v>
       </c>
-      <c r="F18" s="20"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="V18" s="1"/>
@@ -2026,7 +2026,7 @@
       <c r="C19" s="3">
         <v>90</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>47</v>
       </c>
       <c r="G19" s="3">
@@ -2051,7 +2051,7 @@
       <c r="C20" s="3">
         <v>90</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -2076,7 +2076,7 @@
       <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="F21" s="20"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="3"/>
       <c r="H21" s="15"/>
       <c r="V21" s="1"/>
@@ -2097,7 +2097,7 @@
       <c r="C22" s="3">
         <v>20</v>
       </c>
-      <c r="F22" s="20"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="3"/>
       <c r="H22" s="15"/>
       <c r="V22" s="1"/>
@@ -2118,7 +2118,7 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>51</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -2143,7 +2143,7 @@
       <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="3"/>
       <c r="H24" s="15"/>
       <c r="V24" s="1"/>
@@ -2164,7 +2164,7 @@
       <c r="C25" s="3">
         <v>90</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="3">
@@ -2189,7 +2189,7 @@
       <c r="C26" s="3">
         <v>24</v>
       </c>
-      <c r="F26" s="20"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="3"/>
       <c r="H26" s="15"/>
       <c r="V26" s="1"/>
@@ -2210,7 +2210,7 @@
       <c r="C27" s="3">
         <v>25</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>53</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -2235,7 +2235,7 @@
       <c r="C28" s="3">
         <v>26</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>54</v>
       </c>
       <c r="G28" s="3">
@@ -2260,7 +2260,7 @@
       <c r="C29" s="3">
         <v>27</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G29" s="3">
@@ -2285,7 +2285,7 @@
       <c r="C30" s="3">
         <v>28</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="19" t="s">
         <v>57</v>
       </c>
       <c r="G30" s="3">
@@ -2313,7 +2313,7 @@
       <c r="C31" s="3">
         <v>29</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>62</v>
       </c>
       <c r="G31" s="3">
@@ -2340,7 +2340,7 @@
       <c r="C32" s="3">
         <v>30</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>66</v>
       </c>
       <c r="G32" s="3">
@@ -2367,7 +2367,7 @@
       <c r="C33" s="3">
         <v>90</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="19" t="s">
         <v>67</v>
       </c>
       <c r="G33" s="3">
@@ -2395,7 +2395,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="19" t="s">
         <v>68</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -2422,7 +2422,7 @@
       <c r="C35" s="3">
         <v>33</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="19" t="s">
         <v>69</v>
       </c>
       <c r="G35" s="3">
@@ -2450,7 +2450,7 @@
         <v>34</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="19" t="s">
         <v>70</v>
       </c>
       <c r="G36" s="3">
@@ -2477,7 +2477,7 @@
       <c r="C37" s="3">
         <v>35</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="19" t="s">
         <v>79</v>
       </c>
       <c r="G37" s="3">
@@ -2504,7 +2504,7 @@
       <c r="C38" s="3">
         <v>36</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="19" t="s">
         <v>80</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -2531,7 +2531,7 @@
       <c r="C39" s="3">
         <v>90</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="19" t="s">
         <v>81</v>
       </c>
       <c r="G39" s="3">
@@ -2558,7 +2558,7 @@
       <c r="C40" s="3">
         <v>90</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="19" t="s">
         <v>82</v>
       </c>
       <c r="G40" s="3">
@@ -2585,7 +2585,7 @@
       <c r="C41" s="3">
         <v>90</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="19" t="s">
         <v>58</v>
       </c>
       <c r="G41" s="3">
@@ -2612,7 +2612,7 @@
       <c r="C42" s="3">
         <v>90</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="19" t="s">
         <v>71</v>
       </c>
       <c r="G42" s="3">
@@ -2639,7 +2639,7 @@
       <c r="C43" s="3">
         <v>90</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="19" t="s">
         <v>83</v>
       </c>
       <c r="G43" s="3">
@@ -2666,7 +2666,7 @@
       <c r="C44" s="3">
         <v>90</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="19" t="s">
         <v>85</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -2694,7 +2694,7 @@
         <v>43</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="20"/>
+      <c r="F45" s="19"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
         <v>141</v>
@@ -2717,7 +2717,7 @@
       <c r="C46" s="3">
         <v>44</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="19" t="s">
         <v>86</v>
       </c>
       <c r="G46" s="3">
@@ -2745,7 +2745,7 @@
         <v>45</v>
       </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="20" t="s">
+      <c r="F47" s="19" t="s">
         <v>87</v>
       </c>
       <c r="G47" s="3">
@@ -2772,7 +2772,7 @@
       <c r="C48" s="3">
         <v>46</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="19" t="s">
         <v>88</v>
       </c>
       <c r="G48" s="3">
@@ -2799,7 +2799,7 @@
       <c r="C49" s="3">
         <v>90</v>
       </c>
-      <c r="F49" s="20" t="s">
+      <c r="F49" s="19" t="s">
         <v>89</v>
       </c>
       <c r="G49" s="3" t="s">
@@ -2826,7 +2826,7 @@
       <c r="C50" s="3">
         <v>48</v>
       </c>
-      <c r="F50" s="20" t="s">
+      <c r="F50" s="19" t="s">
         <v>90</v>
       </c>
       <c r="G50" s="3">
@@ -2853,7 +2853,7 @@
       <c r="C51" s="3">
         <v>49</v>
       </c>
-      <c r="F51" s="20" t="s">
+      <c r="F51" s="19" t="s">
         <v>91</v>
       </c>
       <c r="G51" s="3">
@@ -2880,7 +2880,7 @@
       <c r="C52" s="3">
         <v>50</v>
       </c>
-      <c r="F52" s="20" t="s">
+      <c r="F52" s="19" t="s">
         <v>63</v>
       </c>
       <c r="G52" s="3">
@@ -2907,7 +2907,7 @@
       <c r="C53" s="3">
         <v>90</v>
       </c>
-      <c r="F53" s="20" t="s">
+      <c r="F53" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G53" s="3">
@@ -2935,7 +2935,7 @@
         <v>52</v>
       </c>
       <c r="E54" s="2"/>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="19" t="s">
         <v>92</v>
       </c>
       <c r="G54" s="3">
@@ -2965,7 +2965,7 @@
       <c r="C55" s="3">
         <v>90</v>
       </c>
-      <c r="F55" s="20" t="s">
+      <c r="F55" s="19" t="s">
         <v>93</v>
       </c>
       <c r="G55" s="3">
@@ -2996,7 +2996,7 @@
         <v>54</v>
       </c>
       <c r="E56" s="2"/>
-      <c r="F56" s="20" t="s">
+      <c r="F56" s="19" t="s">
         <v>94</v>
       </c>
       <c r="G56" s="3">
@@ -3026,7 +3026,7 @@
       <c r="C57" s="3">
         <v>55</v>
       </c>
-      <c r="F57" s="20" t="s">
+      <c r="F57" s="19" t="s">
         <v>95</v>
       </c>
       <c r="G57" s="3">
@@ -3053,7 +3053,7 @@
       <c r="C58" s="3">
         <v>56</v>
       </c>
-      <c r="F58" s="20" t="s">
+      <c r="F58" s="19" t="s">
         <v>96</v>
       </c>
       <c r="G58" s="3">
@@ -3080,7 +3080,7 @@
       <c r="C59" s="3">
         <v>57</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F59" s="19" t="s">
         <v>97</v>
       </c>
       <c r="G59" s="3" t="s">
@@ -3107,7 +3107,7 @@
       <c r="C60" s="3">
         <v>58</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="19" t="s">
         <v>98</v>
       </c>
       <c r="G60" s="3">
@@ -3134,7 +3134,7 @@
       <c r="C61" s="3">
         <v>59</v>
       </c>
-      <c r="F61" s="20" t="s">
+      <c r="F61" s="19" t="s">
         <v>99</v>
       </c>
       <c r="G61" s="3">
@@ -3162,7 +3162,7 @@
         <v>90</v>
       </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="19" t="s">
         <v>64</v>
       </c>
       <c r="G62" s="3">
@@ -3184,7 +3184,7 @@
       <c r="C63" s="3">
         <v>61</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F63" s="19" t="s">
         <v>72</v>
       </c>
       <c r="G63" s="3">
@@ -3205,7 +3205,7 @@
       <c r="C64" s="3">
         <v>62</v>
       </c>
-      <c r="F64" s="20" t="s">
+      <c r="F64" s="19" t="s">
         <v>60</v>
       </c>
       <c r="G64" s="3">
@@ -3226,7 +3226,7 @@
       <c r="C65" s="3">
         <v>63</v>
       </c>
-      <c r="F65" s="20" t="s">
+      <c r="F65" s="19" t="s">
         <v>100</v>
       </c>
       <c r="G65" s="3" t="s">
@@ -3247,7 +3247,7 @@
       <c r="C66" s="3">
         <v>64</v>
       </c>
-      <c r="F66" s="20" t="s">
+      <c r="F66" s="19" t="s">
         <v>101</v>
       </c>
       <c r="G66" s="3">
@@ -3268,7 +3268,7 @@
       <c r="C67" s="3">
         <v>65</v>
       </c>
-      <c r="F67" s="20" t="s">
+      <c r="F67" s="19" t="s">
         <v>102</v>
       </c>
       <c r="G67" s="3">
@@ -3290,7 +3290,7 @@
         <v>66</v>
       </c>
       <c r="E68" s="2"/>
-      <c r="F68" s="20" t="s">
+      <c r="F68" s="19" t="s">
         <v>103</v>
       </c>
       <c r="G68" s="3">
@@ -3311,7 +3311,7 @@
       <c r="C69" s="3">
         <v>90</v>
       </c>
-      <c r="F69" s="20" t="s">
+      <c r="F69" s="19" t="s">
         <v>104</v>
       </c>
       <c r="G69" s="3" t="s">
@@ -3332,7 +3332,7 @@
       <c r="C70" s="3">
         <v>68</v>
       </c>
-      <c r="F70" s="20"/>
+      <c r="F70" s="19"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3" t="s">
         <v>123</v>
@@ -3349,7 +3349,7 @@
       <c r="C71" s="3">
         <v>69</v>
       </c>
-      <c r="F71" s="20" t="s">
+      <c r="F71" s="19" t="s">
         <v>105</v>
       </c>
       <c r="G71" s="3">
@@ -3370,7 +3370,7 @@
       <c r="C72" s="3">
         <v>70</v>
       </c>
-      <c r="F72" s="20" t="s">
+      <c r="F72" s="19" t="s">
         <v>106</v>
       </c>
       <c r="G72" s="3">
@@ -3391,7 +3391,7 @@
       <c r="C73" s="3">
         <v>71</v>
       </c>
-      <c r="F73" s="20" t="s">
+      <c r="F73" s="19" t="s">
         <v>65</v>
       </c>
       <c r="G73" s="3">
@@ -3412,7 +3412,7 @@
       <c r="C74" s="3">
         <v>72</v>
       </c>
-      <c r="F74" s="20" t="s">
+      <c r="F74" s="19" t="s">
         <v>73</v>
       </c>
       <c r="G74" s="3">
@@ -3433,7 +3433,7 @@
       <c r="C75" s="3">
         <v>73</v>
       </c>
-      <c r="F75" s="20" t="s">
+      <c r="F75" s="19" t="s">
         <v>107</v>
       </c>
       <c r="G75" s="3">
@@ -3454,7 +3454,7 @@
       <c r="C76" s="3">
         <v>90</v>
       </c>
-      <c r="F76" s="20" t="s">
+      <c r="F76" s="19" t="s">
         <v>61</v>
       </c>
       <c r="G76" s="3">
@@ -3475,7 +3475,7 @@
       <c r="C77" s="3">
         <v>75</v>
       </c>
-      <c r="F77" s="20" t="s">
+      <c r="F77" s="19" t="s">
         <v>108</v>
       </c>
       <c r="G77" s="3">

</xml_diff>